<commit_message>
Document updated (which to exclude)
</commit_message>
<xml_diff>
--- a/data/tbi_pecarn/TBI PUD Documentation 10-08-2013.xlsx
+++ b/data/tbi_pecarn/TBI PUD Documentation 10-08-2013.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyunsuk\STAT215A\stat-215-a\rule-vetting\data\tbi_pecarn\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="450" windowWidth="20835" windowHeight="8670"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="344">
   <si>
     <t>Dataset Programs</t>
   </si>
@@ -697,7 +702,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -707,7 +712,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -725,7 +730,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -735,7 +740,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -755,7 +760,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -764,7 +769,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -796,7 +801,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -806,7 +811,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -831,7 +836,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -841,7 +846,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -859,7 +864,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -869,7 +874,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -886,7 +891,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -896,7 +901,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -914,7 +919,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -924,7 +929,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -941,7 +946,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -951,7 +956,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -969,7 +974,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -979,7 +984,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -996,7 +1001,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1006,7 +1011,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1024,7 +1029,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1034,7 +1039,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1051,7 +1056,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1061,7 +1066,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1078,7 +1083,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1088,7 +1093,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1106,7 +1111,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1116,7 +1121,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1139,7 +1144,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1149,7 +1154,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1164,7 +1169,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1174,7 +1179,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1191,7 +1196,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1201,7 +1206,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1218,7 +1223,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1228,7 +1233,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1243,7 +1248,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1253,7 +1258,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1268,7 +1273,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1278,7 +1283,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1293,7 +1298,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1303,7 +1308,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1322,7 +1327,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1332,7 +1337,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1384,7 +1389,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1394,7 +1399,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1410,7 +1415,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1420,7 +1425,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1436,7 +1441,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1446,7 +1451,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1461,7 +1466,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1471,7 +1476,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1487,7 +1492,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1497,7 +1502,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1513,7 +1518,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1523,7 +1528,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1537,7 +1542,7 @@
       <rPr>
         <b/>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1546,7 +1551,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1602,7 +1607,7 @@
         <i/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1612,7 +1617,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="맑은 고딕"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1771,16 +1776,93 @@
 Medium
       Any other mechanism</t>
   </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>back</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>back</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>exclude 3-13
+(only 969)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aaron</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>RES</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>RES</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>RES</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>RES</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAIN RES</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1788,7 +1870,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1796,20 +1878,20 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1817,14 +1899,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1832,8 +1914,15 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1927,7 +2016,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2070,9 +2159,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2080,12 +2172,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2127,7 +2222,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2162,7 +2257,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2371,22 +2466,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D352"/>
+  <dimension ref="A1:F352"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" style="18" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" style="19" customWidth="1"/>
+    <col min="1" max="1" width="25.75" style="18" customWidth="1"/>
+    <col min="2" max="2" width="47.75" style="19" customWidth="1"/>
     <col min="3" max="3" width="37" style="18" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" style="20" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="48.125" style="20" customWidth="1"/>
+    <col min="5" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -2394,7 +2489,7 @@
       <c r="C1" s="43"/>
       <c r="D1" s="44"/>
     </row>
-    <row r="2" spans="1:4" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>158</v>
       </c>
@@ -2404,7 +2499,7 @@
       <c r="C2" s="37"/>
       <c r="D2" s="37"/>
     </row>
-    <row r="3" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>320</v>
       </c>
@@ -2414,7 +2509,7 @@
       <c r="C3" s="41"/>
       <c r="D3" s="41"/>
     </row>
-    <row r="4" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>159</v>
       </c>
@@ -2424,7 +2519,7 @@
       <c r="C4" s="41"/>
       <c r="D4" s="41"/>
     </row>
-    <row r="5" spans="1:4" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>162</v>
       </c>
@@ -2434,7 +2529,7 @@
       <c r="C5" s="46"/>
       <c r="D5" s="47"/>
     </row>
-    <row r="6" spans="1:4" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>161</v>
       </c>
@@ -2444,7 +2539,7 @@
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
     </row>
-    <row r="7" spans="1:4" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>278</v>
       </c>
@@ -2454,7 +2549,7 @@
       <c r="C7" s="37"/>
       <c r="D7" s="37"/>
     </row>
-    <row r="8" spans="1:4" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>279</v>
       </c>
@@ -2464,19 +2559,19 @@
       <c r="C8" s="39"/>
       <c r="D8" s="40"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="29"/>
       <c r="B9" s="30"/>
       <c r="C9" s="29"/>
       <c r="D9" s="31"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="2"/>
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>1</v>
       </c>
@@ -2490,7 +2585,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>258</v>
       </c>
@@ -2503,8 +2598,11 @@
       <c r="D12" s="7" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="99" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>3</v>
       </c>
@@ -2517,8 +2615,11 @@
       <c r="D13" s="7" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="99" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>4</v>
       </c>
@@ -2529,8 +2630,11 @@
         <v>224</v>
       </c>
       <c r="D14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" ht="315" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="346.5" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>323</v>
       </c>
@@ -2542,7 +2646,7 @@
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" ht="240" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="264" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>272</v>
       </c>
@@ -2556,7 +2660,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="10" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="10" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>6</v>
       </c>
@@ -2570,7 +2674,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>7</v>
       </c>
@@ -2582,7 +2686,7 @@
       </c>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="99" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>8</v>
       </c>
@@ -2596,7 +2700,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>9</v>
       </c>
@@ -2608,7 +2712,7 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>10</v>
       </c>
@@ -2622,7 +2726,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="99" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>12</v>
       </c>
@@ -2636,7 +2740,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>14</v>
       </c>
@@ -2648,7 +2752,7 @@
       </c>
       <c r="D23" s="7"/>
     </row>
-    <row r="24" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>15</v>
       </c>
@@ -2662,7 +2766,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>16</v>
       </c>
@@ -2676,7 +2780,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="99" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>17</v>
       </c>
@@ -2690,7 +2794,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>18</v>
       </c>
@@ -2702,7 +2806,7 @@
       </c>
       <c r="D27" s="7"/>
     </row>
-    <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>19</v>
       </c>
@@ -2716,7 +2820,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="99" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>20</v>
       </c>
@@ -2730,7 +2834,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>21</v>
       </c>
@@ -2744,7 +2848,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>22</v>
       </c>
@@ -2755,8 +2859,11 @@
         <v>263</v>
       </c>
       <c r="D31" s="7"/>
-    </row>
-    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E31" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>23</v>
       </c>
@@ -2768,7 +2875,7 @@
       </c>
       <c r="D32" s="7"/>
     </row>
-    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>24</v>
       </c>
@@ -2780,7 +2887,7 @@
       </c>
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>25</v>
       </c>
@@ -2792,7 +2899,7 @@
       </c>
       <c r="D34" s="7"/>
     </row>
-    <row r="35" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>26</v>
       </c>
@@ -2803,8 +2910,11 @@
         <v>239</v>
       </c>
       <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>27</v>
       </c>
@@ -2815,8 +2925,11 @@
         <v>240</v>
       </c>
       <c r="D36" s="7"/>
-    </row>
-    <row r="37" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="E36" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="132" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>28</v>
       </c>
@@ -2827,8 +2940,11 @@
         <v>241</v>
       </c>
       <c r="D37" s="7"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>29</v>
       </c>
@@ -2840,7 +2956,7 @@
       </c>
       <c r="D38" s="21"/>
     </row>
-    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>31</v>
       </c>
@@ -2851,8 +2967,14 @@
         <v>243</v>
       </c>
       <c r="D39" s="7"/>
-    </row>
-    <row r="40" spans="1:4" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="E39" s="48" t="s">
+        <v>329</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>33</v>
       </c>
@@ -2866,7 +2988,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>34</v>
       </c>
@@ -2880,7 +3002,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="66" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>35</v>
       </c>
@@ -2894,7 +3016,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="66" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>36</v>
       </c>
@@ -2908,7 +3030,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="44" spans="1:4" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>37</v>
       </c>
@@ -2922,7 +3044,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="45" spans="1:4" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>38</v>
       </c>
@@ -2936,7 +3058,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="99" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>39</v>
       </c>
@@ -2950,7 +3072,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="66" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>41</v>
       </c>
@@ -2964,7 +3086,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>42</v>
       </c>
@@ -2976,7 +3098,7 @@
       </c>
       <c r="D48" s="7"/>
     </row>
-    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>44</v>
       </c>
@@ -2988,7 +3110,7 @@
       </c>
       <c r="D49" s="7"/>
     </row>
-    <row r="50" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>45</v>
       </c>
@@ -3002,7 +3124,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>46</v>
       </c>
@@ -3016,7 +3138,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>47</v>
       </c>
@@ -3030,7 +3152,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>48</v>
       </c>
@@ -3044,7 +3166,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>49</v>
       </c>
@@ -3058,7 +3180,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>50</v>
       </c>
@@ -3070,7 +3192,7 @@
       </c>
       <c r="D55" s="7"/>
     </row>
-    <row r="56" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>51</v>
       </c>
@@ -3084,7 +3206,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>53</v>
       </c>
@@ -3098,7 +3220,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>55</v>
       </c>
@@ -3110,7 +3232,7 @@
       </c>
       <c r="D58" s="7"/>
     </row>
-    <row r="59" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>56</v>
       </c>
@@ -3124,7 +3246,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>57</v>
       </c>
@@ -3138,7 +3260,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>58</v>
       </c>
@@ -3152,7 +3274,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>59</v>
       </c>
@@ -3166,7 +3288,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>60</v>
       </c>
@@ -3180,7 +3302,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>61</v>
       </c>
@@ -3194,7 +3316,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>62</v>
       </c>
@@ -3206,7 +3328,7 @@
       </c>
       <c r="D65" s="7"/>
     </row>
-    <row r="66" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>63</v>
       </c>
@@ -3220,7 +3342,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>64</v>
       </c>
@@ -3234,7 +3356,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>65</v>
       </c>
@@ -3248,7 +3370,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>66</v>
       </c>
@@ -3262,7 +3384,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
         <v>67</v>
       </c>
@@ -3276,7 +3398,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>68</v>
       </c>
@@ -3288,7 +3410,7 @@
       </c>
       <c r="D71" s="7"/>
     </row>
-    <row r="72" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>70</v>
       </c>
@@ -3302,7 +3424,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
         <v>71</v>
       </c>
@@ -3316,7 +3438,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
         <v>72</v>
       </c>
@@ -3330,7 +3452,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
         <v>73</v>
       </c>
@@ -3344,7 +3466,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A76" s="12" t="s">
         <v>74</v>
       </c>
@@ -3358,7 +3480,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A77" s="12" t="s">
         <v>75</v>
       </c>
@@ -3372,7 +3494,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A78" s="12" t="s">
         <v>76</v>
       </c>
@@ -3386,7 +3508,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
         <v>77</v>
       </c>
@@ -3398,7 +3520,7 @@
       </c>
       <c r="D79" s="7"/>
     </row>
-    <row r="80" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="132" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
         <v>78</v>
       </c>
@@ -3411,8 +3533,11 @@
       <c r="D80" s="6" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" s="33" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E80" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A81" s="34" t="s">
         <v>285</v>
       </c>
@@ -3425,8 +3550,11 @@
       <c r="D81" s="35" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" s="33" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E81" s="33" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A82" s="34" t="s">
         <v>288</v>
       </c>
@@ -3439,8 +3567,11 @@
       <c r="D82" s="35" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" s="33" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E82" s="33" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A83" s="34" t="s">
         <v>290</v>
       </c>
@@ -3453,8 +3584,11 @@
       <c r="D83" s="35" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" s="33" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E83" s="33" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A84" s="34" t="s">
         <v>292</v>
       </c>
@@ -3467,8 +3601,11 @@
       <c r="D84" s="35" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" s="33" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E84" s="33" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A85" s="34" t="s">
         <v>294</v>
       </c>
@@ -3481,8 +3618,11 @@
       <c r="D85" s="35" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" s="33" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E85" s="33" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A86" s="34" t="s">
         <v>296</v>
       </c>
@@ -3495,8 +3635,11 @@
       <c r="D86" s="35" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" s="33" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E86" s="33" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A87" s="34" t="s">
         <v>298</v>
       </c>
@@ -3509,8 +3652,11 @@
       <c r="D87" s="35" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" s="33" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E87" s="33" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A88" s="34" t="s">
         <v>300</v>
       </c>
@@ -3523,8 +3669,11 @@
       <c r="D88" s="35" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" s="33" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E88" s="33" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A89" s="34" t="s">
         <v>302</v>
       </c>
@@ -3537,8 +3686,11 @@
       <c r="D89" s="35" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" s="33" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E89" s="33" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A90" s="34" t="s">
         <v>304</v>
       </c>
@@ -3551,8 +3703,11 @@
       <c r="D90" s="35" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" s="33" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E90" s="33" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A91" s="34" t="s">
         <v>306</v>
       </c>
@@ -3565,8 +3720,11 @@
       <c r="D91" s="35" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" s="33" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E91" s="33" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A92" s="34" t="s">
         <v>308</v>
       </c>
@@ -3579,8 +3737,11 @@
       <c r="D92" s="35" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" s="33" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E92" s="33" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A93" s="34" t="s">
         <v>310</v>
       </c>
@@ -3593,8 +3754,11 @@
       <c r="D93" s="35" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" s="33" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E93" s="33" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A94" s="34" t="s">
         <v>312</v>
       </c>
@@ -3607,8 +3771,11 @@
       <c r="D94" s="35" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" s="33" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E94" s="33" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A95" s="34" t="s">
         <v>314</v>
       </c>
@@ -3621,8 +3788,11 @@
       <c r="D95" s="35" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" s="33" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="E95" s="33" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A96" s="34" t="s">
         <v>316</v>
       </c>
@@ -3635,8 +3805,11 @@
       <c r="D96" s="35" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E96" s="33" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
         <v>79</v>
       </c>
@@ -3649,8 +3822,11 @@
       <c r="D97" s="7" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="E97" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
         <v>80</v>
       </c>
@@ -3663,8 +3839,11 @@
       <c r="D98" s="7" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="E98" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
         <v>81</v>
       </c>
@@ -3677,8 +3856,11 @@
       <c r="D99" s="7" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="E99" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
         <v>82</v>
       </c>
@@ -3691,8 +3873,11 @@
       <c r="D100" s="7" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="E100" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
         <v>83</v>
       </c>
@@ -3705,8 +3890,11 @@
       <c r="D101" s="7" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="E101" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
         <v>84</v>
       </c>
@@ -3720,7 +3908,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="103" spans="1:4" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
         <v>86</v>
       </c>
@@ -3734,7 +3922,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="104" spans="1:4" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
         <v>87</v>
       </c>
@@ -3748,7 +3936,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
         <v>89</v>
       </c>
@@ -3760,7 +3948,7 @@
       </c>
       <c r="D105" s="7"/>
     </row>
-    <row r="106" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
         <v>90</v>
       </c>
@@ -3773,8 +3961,11 @@
       <c r="D106" s="7" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="E106" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
         <v>91</v>
       </c>
@@ -3787,8 +3978,11 @@
       <c r="D107" s="7" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E107" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
         <v>92</v>
       </c>
@@ -3799,8 +3993,11 @@
         <v>267</v>
       </c>
       <c r="D108" s="7"/>
-    </row>
-    <row r="109" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="E108" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
         <v>93</v>
       </c>
@@ -3811,8 +4008,11 @@
         <v>250</v>
       </c>
       <c r="D109" s="15"/>
-    </row>
-    <row r="110" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E109" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
         <v>95</v>
       </c>
@@ -3825,8 +4025,11 @@
       <c r="D110" s="7" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E110" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
         <v>96</v>
       </c>
@@ -3839,8 +4042,11 @@
       <c r="D111" s="7" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="E111" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="132" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
         <v>97</v>
       </c>
@@ -3853,8 +4059,11 @@
       <c r="D112" s="7" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E112" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
         <v>99</v>
       </c>
@@ -3867,8 +4076,11 @@
       <c r="D113" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E113" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
         <v>100</v>
       </c>
@@ -3881,8 +4093,11 @@
       <c r="D114" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E114" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
         <v>101</v>
       </c>
@@ -3895,8 +4110,11 @@
       <c r="D115" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E115" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
         <v>102</v>
       </c>
@@ -3909,8 +4127,11 @@
       <c r="D116" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E116" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
         <v>103</v>
       </c>
@@ -3923,8 +4144,11 @@
       <c r="D117" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E117" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
         <v>104</v>
       </c>
@@ -3937,8 +4161,11 @@
       <c r="D118" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E118" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
         <v>105</v>
       </c>
@@ -3951,8 +4178,11 @@
       <c r="D119" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E119" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
         <v>106</v>
       </c>
@@ -3965,8 +4195,11 @@
       <c r="D120" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E120" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
         <v>107</v>
       </c>
@@ -3979,8 +4212,11 @@
       <c r="D121" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E121" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
         <v>108</v>
       </c>
@@ -3993,8 +4229,11 @@
       <c r="D122" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E122" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
         <v>109</v>
       </c>
@@ -4007,8 +4246,11 @@
       <c r="D123" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E123" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
         <v>110</v>
       </c>
@@ -4021,8 +4263,11 @@
       <c r="D124" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E124" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
         <v>111</v>
       </c>
@@ -4035,8 +4280,11 @@
       <c r="D125" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E125" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
         <v>112</v>
       </c>
@@ -4049,8 +4297,11 @@
       <c r="D126" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E126" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
         <v>212</v>
       </c>
@@ -4063,8 +4314,11 @@
       <c r="D127" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E127" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
         <v>113</v>
       </c>
@@ -4077,8 +4331,11 @@
       <c r="D128" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E128" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
         <v>114</v>
       </c>
@@ -4091,8 +4348,11 @@
       <c r="D129" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E129" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
         <v>269</v>
       </c>
@@ -4105,8 +4365,11 @@
       <c r="D130" s="16" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E130" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
         <v>115</v>
       </c>
@@ -4117,8 +4380,11 @@
         <v>263</v>
       </c>
       <c r="D131" s="7"/>
-    </row>
-    <row r="132" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E131" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
         <v>117</v>
       </c>
@@ -4129,8 +4395,11 @@
         <v>263</v>
       </c>
       <c r="D132" s="7"/>
-    </row>
-    <row r="133" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E132" s="1" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="99" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
         <v>118</v>
       </c>
@@ -4143,8 +4412,11 @@
       <c r="D133" s="7" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E133" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
         <v>119</v>
       </c>
@@ -4155,8 +4427,11 @@
         <v>263</v>
       </c>
       <c r="D134" s="7"/>
-    </row>
-    <row r="135" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E134" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
         <v>120</v>
       </c>
@@ -4167,8 +4442,11 @@
         <v>263</v>
       </c>
       <c r="D135" s="7"/>
-    </row>
-    <row r="136" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="E135" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="99" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
         <v>121</v>
       </c>
@@ -4181,1298 +4459,1301 @@
       <c r="D136" s="7" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E136" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="14"/>
       <c r="B137" s="13"/>
       <c r="C137" s="14"/>
       <c r="D137" s="17"/>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="14"/>
       <c r="B138" s="13"/>
       <c r="C138" s="14"/>
       <c r="D138" s="17"/>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="14"/>
       <c r="B139" s="13"/>
       <c r="C139" s="14"/>
       <c r="D139" s="17"/>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="14"/>
       <c r="B140" s="13"/>
       <c r="C140" s="14"/>
       <c r="D140" s="17"/>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="14"/>
       <c r="B141" s="13"/>
       <c r="C141" s="14"/>
       <c r="D141" s="17"/>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="14"/>
       <c r="B142" s="13"/>
       <c r="C142" s="14"/>
       <c r="D142" s="17"/>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="14"/>
       <c r="B143" s="13"/>
       <c r="C143" s="14"/>
       <c r="D143" s="17"/>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="14"/>
       <c r="B144" s="13"/>
       <c r="C144" s="14"/>
       <c r="D144" s="17"/>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="14"/>
       <c r="B145" s="13"/>
       <c r="C145" s="14"/>
       <c r="D145" s="17"/>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="14"/>
       <c r="B146" s="13"/>
       <c r="C146" s="14"/>
       <c r="D146" s="17"/>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="14"/>
       <c r="B147" s="13"/>
       <c r="C147" s="14"/>
       <c r="D147" s="17"/>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="14"/>
       <c r="B148" s="13"/>
       <c r="C148" s="14"/>
       <c r="D148" s="17"/>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="14"/>
       <c r="B149" s="13"/>
       <c r="C149" s="14"/>
       <c r="D149" s="17"/>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="14"/>
       <c r="B150" s="13"/>
       <c r="C150" s="14"/>
       <c r="D150" s="17"/>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="14"/>
       <c r="B151" s="13"/>
       <c r="C151" s="14"/>
       <c r="D151" s="17"/>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="14"/>
       <c r="B152" s="13"/>
       <c r="C152" s="14"/>
       <c r="D152" s="17"/>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="14"/>
       <c r="B153" s="13"/>
       <c r="C153" s="14"/>
       <c r="D153" s="17"/>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="14"/>
       <c r="B154" s="13"/>
       <c r="C154" s="14"/>
       <c r="D154" s="17"/>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="14"/>
       <c r="B155" s="13"/>
       <c r="C155" s="14"/>
       <c r="D155" s="17"/>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="14"/>
       <c r="B156" s="13"/>
       <c r="C156" s="14"/>
       <c r="D156" s="17"/>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="14"/>
       <c r="B157" s="13"/>
       <c r="C157" s="14"/>
       <c r="D157" s="17"/>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="14"/>
       <c r="B158" s="13"/>
       <c r="C158" s="14"/>
       <c r="D158" s="17"/>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="14"/>
       <c r="B159" s="13"/>
       <c r="C159" s="14"/>
       <c r="D159" s="17"/>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="14"/>
       <c r="B160" s="13"/>
       <c r="C160" s="14"/>
       <c r="D160" s="17"/>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="14"/>
       <c r="B161" s="13"/>
       <c r="C161" s="14"/>
       <c r="D161" s="17"/>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="14"/>
       <c r="B162" s="13"/>
       <c r="C162" s="14"/>
       <c r="D162" s="17"/>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="14"/>
       <c r="B163" s="13"/>
       <c r="C163" s="14"/>
       <c r="D163" s="17"/>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="14"/>
       <c r="B164" s="13"/>
       <c r="C164" s="14"/>
       <c r="D164" s="17"/>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="14"/>
       <c r="B165" s="13"/>
       <c r="C165" s="14"/>
       <c r="D165" s="17"/>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="14"/>
       <c r="B166" s="13"/>
       <c r="C166" s="14"/>
       <c r="D166" s="17"/>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="14"/>
       <c r="B167" s="13"/>
       <c r="C167" s="14"/>
       <c r="D167" s="17"/>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="14"/>
       <c r="B168" s="13"/>
       <c r="C168" s="14"/>
       <c r="D168" s="17"/>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="14"/>
       <c r="B169" s="13"/>
       <c r="C169" s="14"/>
       <c r="D169" s="17"/>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" s="14"/>
       <c r="B170" s="13"/>
       <c r="C170" s="14"/>
       <c r="D170" s="17"/>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="14"/>
       <c r="B171" s="13"/>
       <c r="C171" s="14"/>
       <c r="D171" s="17"/>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="14"/>
       <c r="B172" s="13"/>
       <c r="C172" s="14"/>
       <c r="D172" s="17"/>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="14"/>
       <c r="B173" s="13"/>
       <c r="C173" s="14"/>
       <c r="D173" s="17"/>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" s="14"/>
       <c r="B174" s="13"/>
       <c r="C174" s="14"/>
       <c r="D174" s="17"/>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="14"/>
       <c r="B175" s="13"/>
       <c r="C175" s="14"/>
       <c r="D175" s="17"/>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="14"/>
       <c r="B176" s="13"/>
       <c r="C176" s="14"/>
       <c r="D176" s="17"/>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="14"/>
       <c r="B177" s="13"/>
       <c r="C177" s="14"/>
       <c r="D177" s="17"/>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="14"/>
       <c r="B178" s="13"/>
       <c r="C178" s="14"/>
       <c r="D178" s="17"/>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="14"/>
       <c r="B179" s="13"/>
       <c r="C179" s="14"/>
       <c r="D179" s="17"/>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="14"/>
       <c r="B180" s="13"/>
       <c r="C180" s="14"/>
       <c r="D180" s="17"/>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="14"/>
       <c r="B181" s="13"/>
       <c r="C181" s="14"/>
       <c r="D181" s="17"/>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="14"/>
       <c r="B182" s="13"/>
       <c r="C182" s="14"/>
       <c r="D182" s="17"/>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="14"/>
       <c r="B183" s="13"/>
       <c r="C183" s="14"/>
       <c r="D183" s="17"/>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="14"/>
       <c r="B184" s="13"/>
       <c r="C184" s="14"/>
       <c r="D184" s="17"/>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="14"/>
       <c r="B185" s="13"/>
       <c r="C185" s="14"/>
       <c r="D185" s="17"/>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="14"/>
       <c r="B186" s="13"/>
       <c r="C186" s="14"/>
       <c r="D186" s="17"/>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="14"/>
       <c r="B187" s="13"/>
       <c r="C187" s="14"/>
       <c r="D187" s="17"/>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="14"/>
       <c r="B188" s="13"/>
       <c r="C188" s="14"/>
       <c r="D188" s="17"/>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="14"/>
       <c r="B189" s="13"/>
       <c r="C189" s="14"/>
       <c r="D189" s="17"/>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="14"/>
       <c r="B190" s="13"/>
       <c r="C190" s="14"/>
       <c r="D190" s="17"/>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="14"/>
       <c r="B191" s="13"/>
       <c r="C191" s="14"/>
       <c r="D191" s="17"/>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="14"/>
       <c r="B192" s="13"/>
       <c r="C192" s="14"/>
       <c r="D192" s="17"/>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="14"/>
       <c r="B193" s="13"/>
       <c r="C193" s="14"/>
       <c r="D193" s="17"/>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="14"/>
       <c r="B194" s="13"/>
       <c r="C194" s="14"/>
       <c r="D194" s="17"/>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="14"/>
       <c r="B195" s="13"/>
       <c r="C195" s="14"/>
       <c r="D195" s="17"/>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="14"/>
       <c r="B196" s="13"/>
       <c r="C196" s="14"/>
       <c r="D196" s="17"/>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="14"/>
       <c r="B197" s="13"/>
       <c r="C197" s="14"/>
       <c r="D197" s="17"/>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="14"/>
       <c r="B198" s="13"/>
       <c r="C198" s="14"/>
       <c r="D198" s="17"/>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="14"/>
       <c r="B199" s="13"/>
       <c r="C199" s="14"/>
       <c r="D199" s="17"/>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="14"/>
       <c r="B200" s="13"/>
       <c r="C200" s="14"/>
       <c r="D200" s="17"/>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="14"/>
       <c r="B201" s="13"/>
       <c r="C201" s="14"/>
       <c r="D201" s="17"/>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" s="14"/>
       <c r="B202" s="13"/>
       <c r="C202" s="14"/>
       <c r="D202" s="17"/>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" s="14"/>
       <c r="B203" s="13"/>
       <c r="C203" s="14"/>
       <c r="D203" s="17"/>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" s="14"/>
       <c r="B204" s="13"/>
       <c r="C204" s="14"/>
       <c r="D204" s="17"/>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" s="14"/>
       <c r="B205" s="13"/>
       <c r="C205" s="14"/>
       <c r="D205" s="17"/>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" s="14"/>
       <c r="B206" s="13"/>
       <c r="C206" s="14"/>
       <c r="D206" s="17"/>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="14"/>
       <c r="B207" s="13"/>
       <c r="C207" s="14"/>
       <c r="D207" s="17"/>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" s="14"/>
       <c r="B208" s="13"/>
       <c r="C208" s="14"/>
       <c r="D208" s="17"/>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" s="14"/>
       <c r="B209" s="13"/>
       <c r="C209" s="14"/>
       <c r="D209" s="17"/>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="14"/>
       <c r="B210" s="13"/>
       <c r="C210" s="14"/>
       <c r="D210" s="17"/>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="14"/>
       <c r="B211" s="13"/>
       <c r="C211" s="14"/>
       <c r="D211" s="17"/>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="14"/>
       <c r="B212" s="13"/>
       <c r="C212" s="14"/>
       <c r="D212" s="17"/>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="14"/>
       <c r="B213" s="13"/>
       <c r="C213" s="14"/>
       <c r="D213" s="17"/>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="14"/>
       <c r="B214" s="13"/>
       <c r="C214" s="14"/>
       <c r="D214" s="17"/>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" s="14"/>
       <c r="B215" s="13"/>
       <c r="C215" s="14"/>
       <c r="D215" s="17"/>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" s="14"/>
       <c r="B216" s="13"/>
       <c r="C216" s="14"/>
       <c r="D216" s="17"/>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" s="14"/>
       <c r="B217" s="13"/>
       <c r="C217" s="14"/>
       <c r="D217" s="17"/>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" s="14"/>
       <c r="B218" s="13"/>
       <c r="C218" s="14"/>
       <c r="D218" s="17"/>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="14"/>
       <c r="B219" s="13"/>
       <c r="C219" s="14"/>
       <c r="D219" s="17"/>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" s="14"/>
       <c r="B220" s="13"/>
       <c r="C220" s="14"/>
       <c r="D220" s="17"/>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" s="14"/>
       <c r="B221" s="13"/>
       <c r="C221" s="14"/>
       <c r="D221" s="17"/>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" s="14"/>
       <c r="B222" s="13"/>
       <c r="C222" s="14"/>
       <c r="D222" s="17"/>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" s="14"/>
       <c r="B223" s="13"/>
       <c r="C223" s="14"/>
       <c r="D223" s="17"/>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" s="14"/>
       <c r="B224" s="13"/>
       <c r="C224" s="14"/>
       <c r="D224" s="17"/>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" s="14"/>
       <c r="B225" s="13"/>
       <c r="C225" s="14"/>
       <c r="D225" s="17"/>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" s="14"/>
       <c r="B226" s="13"/>
       <c r="C226" s="14"/>
       <c r="D226" s="17"/>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" s="14"/>
       <c r="B227" s="13"/>
       <c r="C227" s="14"/>
       <c r="D227" s="17"/>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" s="14"/>
       <c r="B228" s="13"/>
       <c r="C228" s="14"/>
       <c r="D228" s="17"/>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" s="14"/>
       <c r="B229" s="13"/>
       <c r="C229" s="14"/>
       <c r="D229" s="17"/>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" s="14"/>
       <c r="B230" s="13"/>
       <c r="C230" s="14"/>
       <c r="D230" s="17"/>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" s="14"/>
       <c r="B231" s="13"/>
       <c r="C231" s="14"/>
       <c r="D231" s="17"/>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" s="14"/>
       <c r="B232" s="13"/>
       <c r="C232" s="14"/>
       <c r="D232" s="17"/>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" s="14"/>
       <c r="B233" s="13"/>
       <c r="C233" s="14"/>
       <c r="D233" s="17"/>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" s="14"/>
       <c r="B234" s="13"/>
       <c r="C234" s="14"/>
       <c r="D234" s="17"/>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" s="14"/>
       <c r="B235" s="13"/>
       <c r="C235" s="14"/>
       <c r="D235" s="17"/>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" s="14"/>
       <c r="B236" s="13"/>
       <c r="C236" s="14"/>
       <c r="D236" s="17"/>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" s="14"/>
       <c r="B237" s="13"/>
       <c r="C237" s="14"/>
       <c r="D237" s="17"/>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" s="14"/>
       <c r="B238" s="13"/>
       <c r="C238" s="14"/>
       <c r="D238" s="17"/>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" s="14"/>
       <c r="B239" s="13"/>
       <c r="C239" s="14"/>
       <c r="D239" s="17"/>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" s="14"/>
       <c r="B240" s="13"/>
       <c r="C240" s="14"/>
       <c r="D240" s="17"/>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" s="14"/>
       <c r="B241" s="13"/>
       <c r="C241" s="14"/>
       <c r="D241" s="17"/>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" s="14"/>
       <c r="B242" s="13"/>
       <c r="C242" s="14"/>
       <c r="D242" s="17"/>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" s="14"/>
       <c r="B243" s="13"/>
       <c r="C243" s="14"/>
       <c r="D243" s="17"/>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" s="14"/>
       <c r="B244" s="13"/>
       <c r="C244" s="14"/>
       <c r="D244" s="17"/>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" s="14"/>
       <c r="B245" s="13"/>
       <c r="C245" s="14"/>
       <c r="D245" s="17"/>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" s="14"/>
       <c r="B246" s="13"/>
       <c r="C246" s="14"/>
       <c r="D246" s="17"/>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" s="14"/>
       <c r="B247" s="13"/>
       <c r="C247" s="14"/>
       <c r="D247" s="17"/>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" s="14"/>
       <c r="B248" s="13"/>
       <c r="C248" s="14"/>
       <c r="D248" s="17"/>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249" s="14"/>
       <c r="B249" s="13"/>
       <c r="C249" s="14"/>
       <c r="D249" s="17"/>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250" s="14"/>
       <c r="B250" s="13"/>
       <c r="C250" s="14"/>
       <c r="D250" s="17"/>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251" s="14"/>
       <c r="B251" s="13"/>
       <c r="C251" s="14"/>
       <c r="D251" s="17"/>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A252" s="14"/>
       <c r="B252" s="13"/>
       <c r="C252" s="14"/>
       <c r="D252" s="17"/>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253" s="14"/>
       <c r="B253" s="13"/>
       <c r="C253" s="14"/>
       <c r="D253" s="17"/>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254" s="14"/>
       <c r="B254" s="13"/>
       <c r="C254" s="14"/>
       <c r="D254" s="17"/>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A255" s="14"/>
       <c r="B255" s="13"/>
       <c r="C255" s="14"/>
       <c r="D255" s="17"/>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256" s="14"/>
       <c r="B256" s="13"/>
       <c r="C256" s="14"/>
       <c r="D256" s="17"/>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A257" s="14"/>
       <c r="B257" s="13"/>
       <c r="C257" s="14"/>
       <c r="D257" s="17"/>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A258" s="14"/>
       <c r="B258" s="13"/>
       <c r="C258" s="14"/>
       <c r="D258" s="17"/>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A259" s="14"/>
       <c r="B259" s="13"/>
       <c r="C259" s="14"/>
       <c r="D259" s="17"/>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A260" s="14"/>
       <c r="B260" s="13"/>
       <c r="C260" s="14"/>
       <c r="D260" s="17"/>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A261" s="14"/>
       <c r="B261" s="13"/>
       <c r="C261" s="14"/>
       <c r="D261" s="17"/>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A262" s="14"/>
       <c r="B262" s="13"/>
       <c r="C262" s="14"/>
       <c r="D262" s="17"/>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A263" s="14"/>
       <c r="B263" s="13"/>
       <c r="C263" s="14"/>
       <c r="D263" s="17"/>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A264" s="14"/>
       <c r="B264" s="13"/>
       <c r="C264" s="14"/>
       <c r="D264" s="17"/>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A265" s="14"/>
       <c r="B265" s="13"/>
       <c r="C265" s="14"/>
       <c r="D265" s="17"/>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A266" s="14"/>
       <c r="B266" s="13"/>
       <c r="C266" s="14"/>
       <c r="D266" s="17"/>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A267" s="14"/>
       <c r="B267" s="13"/>
       <c r="C267" s="14"/>
       <c r="D267" s="17"/>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A268" s="14"/>
       <c r="B268" s="13"/>
       <c r="C268" s="14"/>
       <c r="D268" s="17"/>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A269" s="14"/>
       <c r="B269" s="13"/>
       <c r="C269" s="14"/>
       <c r="D269" s="17"/>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A270" s="14"/>
       <c r="B270" s="13"/>
       <c r="C270" s="14"/>
       <c r="D270" s="17"/>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A271" s="14"/>
       <c r="B271" s="13"/>
       <c r="C271" s="14"/>
       <c r="D271" s="17"/>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A272" s="14"/>
       <c r="B272" s="13"/>
       <c r="C272" s="14"/>
       <c r="D272" s="17"/>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273" s="14"/>
       <c r="B273" s="13"/>
       <c r="C273" s="14"/>
       <c r="D273" s="17"/>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A274" s="14"/>
       <c r="B274" s="13"/>
       <c r="C274" s="14"/>
       <c r="D274" s="17"/>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A275" s="14"/>
       <c r="B275" s="13"/>
       <c r="C275" s="14"/>
       <c r="D275" s="17"/>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A276" s="14"/>
       <c r="B276" s="13"/>
       <c r="C276" s="14"/>
       <c r="D276" s="17"/>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A277" s="14"/>
       <c r="B277" s="13"/>
       <c r="C277" s="14"/>
       <c r="D277" s="17"/>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A278" s="14"/>
       <c r="B278" s="13"/>
       <c r="C278" s="14"/>
       <c r="D278" s="17"/>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A279" s="14"/>
       <c r="B279" s="13"/>
       <c r="C279" s="14"/>
       <c r="D279" s="17"/>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A280" s="14"/>
       <c r="B280" s="13"/>
       <c r="C280" s="14"/>
       <c r="D280" s="17"/>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A281" s="14"/>
       <c r="B281" s="13"/>
       <c r="C281" s="14"/>
       <c r="D281" s="17"/>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A282" s="14"/>
       <c r="B282" s="13"/>
       <c r="C282" s="14"/>
       <c r="D282" s="17"/>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A283" s="14"/>
       <c r="B283" s="13"/>
       <c r="C283" s="14"/>
       <c r="D283" s="17"/>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A284" s="14"/>
       <c r="B284" s="13"/>
       <c r="C284" s="14"/>
       <c r="D284" s="17"/>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A285" s="14"/>
       <c r="B285" s="13"/>
       <c r="C285" s="14"/>
       <c r="D285" s="17"/>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A286" s="14"/>
       <c r="B286" s="13"/>
       <c r="C286" s="14"/>
       <c r="D286" s="17"/>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A287" s="14"/>
       <c r="B287" s="13"/>
       <c r="C287" s="14"/>
       <c r="D287" s="17"/>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A288" s="14"/>
       <c r="B288" s="13"/>
       <c r="C288" s="14"/>
       <c r="D288" s="17"/>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A289" s="14"/>
       <c r="B289" s="13"/>
       <c r="C289" s="14"/>
       <c r="D289" s="17"/>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A290" s="14"/>
       <c r="B290" s="13"/>
       <c r="C290" s="14"/>
       <c r="D290" s="17"/>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A291" s="14"/>
       <c r="B291" s="13"/>
       <c r="C291" s="14"/>
       <c r="D291" s="17"/>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A292" s="14"/>
       <c r="B292" s="13"/>
       <c r="C292" s="14"/>
       <c r="D292" s="17"/>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A293" s="14"/>
       <c r="B293" s="13"/>
       <c r="C293" s="14"/>
       <c r="D293" s="17"/>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A294" s="14"/>
       <c r="B294" s="13"/>
       <c r="C294" s="14"/>
       <c r="D294" s="17"/>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A295" s="14"/>
       <c r="B295" s="13"/>
       <c r="C295" s="14"/>
       <c r="D295" s="17"/>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A296" s="14"/>
       <c r="B296" s="13"/>
       <c r="C296" s="14"/>
       <c r="D296" s="17"/>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A297" s="14"/>
       <c r="B297" s="13"/>
       <c r="C297" s="14"/>
       <c r="D297" s="17"/>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A298" s="14"/>
       <c r="B298" s="13"/>
       <c r="C298" s="14"/>
       <c r="D298" s="17"/>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A299" s="14"/>
       <c r="B299" s="13"/>
       <c r="C299" s="14"/>
       <c r="D299" s="17"/>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A300" s="14"/>
       <c r="B300" s="13"/>
       <c r="C300" s="14"/>
       <c r="D300" s="17"/>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A301" s="14"/>
       <c r="B301" s="13"/>
       <c r="C301" s="14"/>
       <c r="D301" s="17"/>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A302" s="14"/>
       <c r="B302" s="13"/>
       <c r="C302" s="14"/>
       <c r="D302" s="17"/>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A303" s="14"/>
       <c r="B303" s="13"/>
       <c r="C303" s="14"/>
       <c r="D303" s="17"/>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A304" s="14"/>
       <c r="B304" s="13"/>
       <c r="C304" s="14"/>
       <c r="D304" s="17"/>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A305" s="14"/>
       <c r="B305" s="13"/>
       <c r="C305" s="14"/>
       <c r="D305" s="17"/>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A306" s="14"/>
       <c r="B306" s="13"/>
       <c r="C306" s="14"/>
       <c r="D306" s="17"/>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A307" s="14"/>
       <c r="B307" s="13"/>
       <c r="C307" s="14"/>
       <c r="D307" s="17"/>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A308" s="14"/>
       <c r="B308" s="13"/>
       <c r="C308" s="14"/>
       <c r="D308" s="17"/>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A309" s="14"/>
       <c r="B309" s="13"/>
       <c r="C309" s="14"/>
       <c r="D309" s="17"/>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A310" s="14"/>
       <c r="B310" s="13"/>
       <c r="C310" s="14"/>
       <c r="D310" s="17"/>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A311" s="14"/>
       <c r="B311" s="13"/>
       <c r="C311" s="14"/>
       <c r="D311" s="17"/>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A312" s="14"/>
       <c r="B312" s="13"/>
       <c r="C312" s="14"/>
       <c r="D312" s="17"/>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A313" s="14"/>
       <c r="B313" s="13"/>
       <c r="C313" s="14"/>
       <c r="D313" s="17"/>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A314" s="14"/>
       <c r="B314" s="13"/>
       <c r="C314" s="14"/>
       <c r="D314" s="17"/>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A315" s="14"/>
       <c r="B315" s="13"/>
       <c r="C315" s="14"/>
       <c r="D315" s="17"/>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A316" s="14"/>
       <c r="B316" s="13"/>
       <c r="C316" s="14"/>
       <c r="D316" s="17"/>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A317" s="14"/>
       <c r="B317" s="13"/>
       <c r="C317" s="14"/>
       <c r="D317" s="17"/>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A318" s="14"/>
       <c r="B318" s="13"/>
       <c r="C318" s="14"/>
       <c r="D318" s="17"/>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A319" s="14"/>
       <c r="B319" s="13"/>
       <c r="C319" s="14"/>
       <c r="D319" s="17"/>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A320" s="14"/>
       <c r="B320" s="13"/>
       <c r="C320" s="14"/>
       <c r="D320" s="17"/>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A321" s="14"/>
       <c r="B321" s="13"/>
       <c r="C321" s="14"/>
       <c r="D321" s="17"/>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A322" s="14"/>
       <c r="B322" s="13"/>
       <c r="C322" s="14"/>
       <c r="D322" s="17"/>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A323" s="14"/>
       <c r="B323" s="13"/>
       <c r="C323" s="14"/>
       <c r="D323" s="17"/>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A324" s="14"/>
       <c r="B324" s="13"/>
       <c r="C324" s="14"/>
       <c r="D324" s="17"/>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A325" s="14"/>
       <c r="B325" s="13"/>
       <c r="C325" s="14"/>
       <c r="D325" s="17"/>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A326" s="14"/>
       <c r="B326" s="13"/>
       <c r="C326" s="14"/>
       <c r="D326" s="17"/>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A327" s="14"/>
       <c r="B327" s="13"/>
       <c r="C327" s="14"/>
       <c r="D327" s="17"/>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A328" s="14"/>
       <c r="B328" s="13"/>
       <c r="C328" s="14"/>
       <c r="D328" s="17"/>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A329" s="14"/>
       <c r="B329" s="13"/>
       <c r="C329" s="14"/>
       <c r="D329" s="17"/>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A330" s="14"/>
       <c r="B330" s="13"/>
       <c r="C330" s="14"/>
       <c r="D330" s="17"/>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A331" s="14"/>
       <c r="B331" s="13"/>
       <c r="C331" s="14"/>
       <c r="D331" s="17"/>
     </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A332" s="14"/>
       <c r="B332" s="13"/>
       <c r="C332" s="14"/>
       <c r="D332" s="17"/>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A333" s="14"/>
       <c r="B333" s="13"/>
       <c r="C333" s="14"/>
       <c r="D333" s="17"/>
     </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A334" s="14"/>
       <c r="B334" s="13"/>
       <c r="C334" s="14"/>
       <c r="D334" s="17"/>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A335" s="14"/>
       <c r="B335" s="13"/>
       <c r="C335" s="14"/>
       <c r="D335" s="17"/>
     </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A336" s="14"/>
       <c r="B336" s="13"/>
       <c r="C336" s="14"/>
       <c r="D336" s="17"/>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A337" s="14"/>
       <c r="B337" s="13"/>
       <c r="C337" s="14"/>
       <c r="D337" s="17"/>
     </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A338" s="14"/>
       <c r="B338" s="13"/>
       <c r="C338" s="14"/>
       <c r="D338" s="17"/>
     </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A339" s="14"/>
       <c r="B339" s="13"/>
       <c r="C339" s="14"/>
       <c r="D339" s="17"/>
     </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A340" s="14"/>
       <c r="B340" s="13"/>
       <c r="C340" s="14"/>
       <c r="D340" s="17"/>
     </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A341" s="14"/>
       <c r="B341" s="13"/>
       <c r="C341" s="14"/>
       <c r="D341" s="17"/>
     </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A342" s="14"/>
       <c r="B342" s="13"/>
       <c r="C342" s="14"/>
       <c r="D342" s="17"/>
     </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A343" s="14"/>
       <c r="B343" s="13"/>
       <c r="C343" s="14"/>
       <c r="D343" s="17"/>
     </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A344" s="14"/>
       <c r="B344" s="13"/>
       <c r="C344" s="14"/>
       <c r="D344" s="17"/>
     </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A345" s="14"/>
       <c r="B345" s="13"/>
       <c r="C345" s="14"/>
       <c r="D345" s="17"/>
     </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A346" s="14"/>
       <c r="B346" s="13"/>
       <c r="C346" s="14"/>
       <c r="D346" s="17"/>
     </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A347" s="14"/>
       <c r="B347" s="13"/>
       <c r="C347" s="14"/>
       <c r="D347" s="17"/>
     </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A348" s="14"/>
       <c r="B348" s="13"/>
       <c r="C348" s="14"/>
       <c r="D348" s="17"/>
     </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A349" s="14"/>
       <c r="B349" s="13"/>
       <c r="C349" s="14"/>
       <c r="D349" s="17"/>
     </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A350" s="14"/>
       <c r="B350" s="13"/>
       <c r="C350" s="14"/>
       <c r="D350" s="17"/>
     </row>
-    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A351" s="14"/>
       <c r="B351" s="13"/>
       <c r="C351" s="14"/>
       <c r="D351" s="17"/>
     </row>
-    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A352" s="14"/>
       <c r="B352" s="13"/>
       <c r="C352" s="14"/>
@@ -5489,6 +5770,7 @@
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B5:D5"/>
   </mergeCells>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5502,576 +5784,577 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="23"/>
+    <col min="1" max="16384" width="9.125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="14"/>
       <c r="B1" s="14"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="13"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="14"/>
       <c r="B3" s="13"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
       <c r="B4" s="13"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="14"/>
       <c r="B5" s="13"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="13"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="13"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="13"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="13"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="13"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="13"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="13"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="13"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="13"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="13"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="13"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="13"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="13"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="13"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="13"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="13"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="13"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="13"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="13"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="13"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="14"/>
       <c r="B27" s="13"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="14"/>
       <c r="B28" s="13"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="14"/>
       <c r="B29" s="13"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="14"/>
       <c r="B30" s="13"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="14"/>
       <c r="B31" s="13"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="14"/>
       <c r="B32" s="13"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>
       <c r="B33" s="13"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
       <c r="B34" s="13"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="14"/>
       <c r="B35" s="13"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="14"/>
       <c r="B36" s="13"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="14"/>
       <c r="B37" s="13"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="14"/>
       <c r="B38" s="13"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="14"/>
       <c r="B39" s="13"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="14"/>
       <c r="B40" s="13"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="14"/>
       <c r="B41" s="13"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="14"/>
       <c r="B42" s="13"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="14"/>
       <c r="B43" s="13"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="14"/>
       <c r="B44" s="13"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="14"/>
       <c r="B45" s="13"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="14"/>
       <c r="B46" s="13"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="14"/>
       <c r="B47" s="13"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="14"/>
       <c r="B48" s="13"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="14"/>
       <c r="B49" s="13"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="14"/>
       <c r="B50" s="13"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="14"/>
       <c r="B51" s="13"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="14"/>
       <c r="B52" s="13"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="14"/>
       <c r="B53" s="13"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="14"/>
       <c r="B54" s="13"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="14"/>
       <c r="B55" s="13"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="14"/>
       <c r="B56" s="13"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="14"/>
       <c r="B57" s="13"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="14"/>
       <c r="B58" s="13"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="14"/>
       <c r="B59" s="13"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="14"/>
       <c r="B60" s="13"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="14"/>
       <c r="B61" s="13"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="14"/>
       <c r="B62" s="13"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="14"/>
       <c r="B63" s="13"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="14"/>
       <c r="B64" s="13"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="14"/>
       <c r="B65" s="13"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="14"/>
       <c r="B66" s="13"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="14"/>
       <c r="B67" s="13"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="14"/>
       <c r="B68" s="13"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="14"/>
       <c r="B69" s="13"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="24"/>
       <c r="B70" s="14"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="24"/>
       <c r="B71" s="14"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="24"/>
       <c r="B72" s="14"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="14"/>
       <c r="B73" s="13"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="14"/>
       <c r="B74" s="13"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="14"/>
       <c r="B75" s="13"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="14"/>
       <c r="B76" s="13"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="14"/>
       <c r="B77" s="13"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="14"/>
       <c r="B78" s="13"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="14"/>
       <c r="B79" s="13"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="14"/>
       <c r="B80" s="13"/>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="14"/>
       <c r="B81" s="13"/>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="14"/>
       <c r="B82" s="13"/>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="14"/>
       <c r="B83" s="13"/>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="14"/>
       <c r="B84" s="13"/>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="14"/>
       <c r="B85" s="13"/>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="14"/>
       <c r="B86" s="13"/>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="14"/>
       <c r="B87" s="13"/>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="14"/>
       <c r="B88" s="13"/>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="14"/>
       <c r="B89" s="13"/>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="14"/>
       <c r="B90" s="13"/>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="14"/>
       <c r="B91" s="13"/>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="14"/>
       <c r="B92" s="13"/>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="14"/>
       <c r="B93" s="13"/>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="14"/>
       <c r="B94" s="13"/>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="14"/>
       <c r="B95" s="13"/>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="14"/>
       <c r="B96" s="13"/>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="14"/>
       <c r="B97" s="13"/>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="25"/>
       <c r="B98" s="26"/>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="14"/>
       <c r="B99" s="13"/>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="14"/>
       <c r="B100" s="13"/>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="14"/>
       <c r="B101" s="13"/>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="14"/>
       <c r="B102" s="13"/>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="14"/>
       <c r="B103" s="13"/>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="14"/>
       <c r="B104" s="13"/>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="14"/>
       <c r="B105" s="13"/>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="14"/>
       <c r="B106" s="13"/>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="14"/>
       <c r="B107" s="13"/>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="14"/>
       <c r="B108" s="13"/>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="14"/>
       <c r="B109" s="13"/>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="14"/>
       <c r="B110" s="13"/>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="14"/>
       <c r="B111" s="13"/>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="14"/>
       <c r="B112" s="13"/>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="14"/>
       <c r="B113" s="13"/>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="14"/>
       <c r="B114" s="13"/>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="14"/>
       <c r="B115" s="13"/>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="14"/>
       <c r="B116" s="13"/>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="14"/>
       <c r="B117" s="13"/>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="14"/>
       <c r="B118" s="13"/>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="14"/>
       <c r="B119" s="13"/>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="14"/>
       <c r="B120" s="13"/>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="14"/>
       <c r="B121" s="13"/>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="14"/>
       <c r="B122" s="13"/>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="14"/>
       <c r="B123" s="13"/>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="14"/>
       <c r="B124" s="13"/>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="14"/>
       <c r="B125" s="13"/>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="14"/>
       <c r="B126" s="13"/>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="14"/>
       <c r="B127" s="13"/>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="14"/>
       <c r="B128" s="13"/>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="14"/>
       <c r="B129" s="13"/>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="14"/>
       <c r="B130" s="13"/>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="14"/>
       <c r="B131" s="13"/>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="14"/>
       <c r="B132" s="13"/>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="14"/>
       <c r="B133" s="13"/>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="14"/>
       <c r="B134" s="13"/>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="14"/>
       <c r="B135" s="13"/>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="14"/>
       <c r="B136" s="13"/>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="14"/>
       <c r="B137" s="13"/>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="14"/>
       <c r="B138" s="13"/>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="14"/>
       <c r="B139" s="13"/>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="14"/>
       <c r="B140" s="13"/>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="14"/>
       <c r="B141" s="13"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -6083,8 +6366,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Data cleaned (Imputation complete) + Simple data set (df_simp) created
</commit_message>
<xml_diff>
--- a/data/tbi_pecarn/TBI PUD Documentation 10-08-2013.xlsx
+++ b/data/tbi_pecarn/TBI PUD Documentation 10-08-2013.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="345">
   <si>
     <t>Dataset Programs</t>
   </si>
@@ -35,63 +35,24 @@
     <t>Label/Description</t>
   </si>
   <si>
-    <t>EmplType</t>
-  </si>
-  <si>
-    <t>Certification</t>
-  </si>
-  <si>
     <t>Does the patient have amnesia for the event?</t>
   </si>
   <si>
-    <t>Amnesia_verb</t>
-  </si>
-  <si>
-    <t>LOCSeparate</t>
-  </si>
-  <si>
     <t>LocLen</t>
   </si>
   <si>
-    <t>Seiz</t>
-  </si>
-  <si>
-    <t>SeizOccur</t>
-  </si>
-  <si>
     <t>When did the post-traumatic seizure occur?</t>
   </si>
   <si>
-    <t>SeizLen</t>
-  </si>
-  <si>
     <t>Duration of post-traumatic seizure</t>
   </si>
   <si>
-    <t>ActNorm</t>
-  </si>
-  <si>
     <t>HA_verb</t>
   </si>
   <si>
-    <t>HASeverity</t>
-  </si>
-  <si>
-    <t>HAStart</t>
-  </si>
-  <si>
     <t>Vomit</t>
   </si>
   <si>
-    <t>VomitNbr</t>
-  </si>
-  <si>
-    <t>VomitStart</t>
-  </si>
-  <si>
-    <t>VomitLast</t>
-  </si>
-  <si>
     <t>Dizzy</t>
   </si>
   <si>
@@ -143,18 +104,12 @@
     <t>AMSOth</t>
   </si>
   <si>
-    <t>SFxPalp</t>
-  </si>
-  <si>
     <t>Palpable skull fracture?</t>
   </si>
   <si>
     <t>SFxPalpDepress</t>
   </si>
   <si>
-    <t>FontBulg</t>
-  </si>
-  <si>
     <t>Anterior fontanelle bulging?</t>
   </si>
   <si>
@@ -179,15 +134,9 @@
     <t>Hema</t>
   </si>
   <si>
-    <t>HemaLoc</t>
-  </si>
-  <si>
     <t>Hematoma(s) or swelling(s) location(s) involved</t>
   </si>
   <si>
-    <t>HemaSize</t>
-  </si>
-  <si>
     <t>Size (diameter) of largest hematoma or swelling</t>
   </si>
   <si>
@@ -212,9 +161,6 @@
     <t>ClavTem</t>
   </si>
   <si>
-    <t>NeuroD</t>
-  </si>
-  <si>
     <t>NeuroDMotor</t>
   </si>
   <si>
@@ -257,39 +203,15 @@
     <t>OSIOth</t>
   </si>
   <si>
-    <t>Drugs</t>
-  </si>
-  <si>
     <t>CTForm1</t>
   </si>
   <si>
-    <t>CTSed</t>
-  </si>
-  <si>
-    <t>CTSedAgitate</t>
-  </si>
-  <si>
-    <t>CTSedAge</t>
-  </si>
-  <si>
-    <t>CTSedRqst</t>
-  </si>
-  <si>
-    <t>CTSedOth</t>
-  </si>
-  <si>
     <t>AgeInMonth</t>
   </si>
   <si>
     <t>Age in months</t>
   </si>
   <si>
-    <t>AgeinYears</t>
-  </si>
-  <si>
-    <t>AgeTwoPlus</t>
-  </si>
-  <si>
     <t>Age: &lt; 2 years</t>
   </si>
   <si>
@@ -492,9 +414,6 @@
   </si>
   <si>
     <t>Other (non-head) substantial injury: other</t>
-  </si>
-  <si>
-    <t>Clinical suspicion for alcohol or drug intoxication (not by laboratory testing)?</t>
   </si>
   <si>
     <t>Is a head CT, skull x-ray or head MRI being ordered or obtained?</t>
@@ -754,6 +673,1090 @@
   </si>
   <si>
     <t>Certification of physician completing the form</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>InjSev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1   Low
+2   Moderate
+3   High</t>
+    </r>
+  </si>
+  <si>
+    <t>Severity of injury mechanism</t>
+  </si>
+  <si>
+    <t>Does the parent think the child is acting normally / like themself?</t>
+  </si>
+  <si>
+    <t>Pre-verbal is marked if the patient is too young to speak.  Non-verbal is marked if the patient is intubated or otherwise unable to give an understandable verbal response.  Pre-verbal and non-verbal were determined by the physician.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LocLen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1   &lt; 5 sec
+2   5 sec - &lt; 1 min
+3   1 -5 min
+4   &gt; 5 min
+92 Not applicable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SeizOcc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1   Immediately on contact
+2   Within 30 minutes of injury
+3   &gt; 30 minutes after injury
+92 Not applicable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SeizLen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1  &lt; 1 min
+2   1 - &lt; 5 min
+3   5 - 15 min
+4  &gt; 15 min
+92  Not applicable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HASev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1   Mild (barely noticeable)
+2   Moderate
+3   Severe (intense)
+92 Not applicable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Start</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1  Before head injury
+2  Within 1 hr of event
+3  1 - 4 hrs after event
+4  &gt; 4 hrs after event
+92  Not applicable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>VomEpi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1   Once
+2   Twice
+3   &gt; 2 times
+92 Not applicable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Start</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1   Before head injury
+2   Within 1 hr of event
+3  1 - 4 hrs after event
+4   &gt; 4 hrs after event
+92  Not applicable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>VomLast</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1   &lt; 1 hr before ED evaluation
+2   1 -4 hrs before ED evaluation
+3  &gt; 4 hrs before ED evaluation
+92  Not applicable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GCSEye</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1     None
+2     Pain
+3     Verbal
+4    Spontaneous</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GCSVerbal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1    None
+2    Incomprehensible sounds (moans)
+3    Inappropriate words (cries to pain)
+4    Confused (irritable/cries)
+5    Oriented (coos/babbles)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GCSMotor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1    None
+2    Abnormal extension posturing
+3    Abnormal flexure posturing
+4    Withdraws to pain
+5    Localizes pain (withdraws to touch)
+6    Follow commands (spontaneous
+      movement)</t>
+    </r>
+  </si>
+  <si>
+    <t>Numeric</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GCSGroup</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1   3 - 13
+2  14 - 15</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HemLoc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1  Frontal
+2  Occipital
+3  Parietal/Temporal
+92  Not applicable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HemSz</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1     Small (&lt;1 cm, barely palpable)
+2     Medium (1-3 cm)
+3     Large (&gt;3 cm)
+92   Not applicable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AgeTwo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1   &lt; 2 years
+2   &gt; = 2 years</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gender</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1   Male
+2   Female</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ethn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1  Hispanic
+2   Non-Hispanic</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Race</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1  White
+2  Black
+3  Asian
+4  American Indian/Alaskan Native
+5  Pacific Islander
+90 Other</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Disp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1  Home
+2  OR
+3  Admit - general inpatient
+4  Admit short-stay (&lt; 24 hr)/observation unit
+5  ICU
+6  Transferred to another hospital
+7 AMA
+8  Death in ED
+90  Other</t>
+    </r>
+  </si>
+  <si>
+    <t>Duration of loss of consciousness</t>
+  </si>
+  <si>
+    <t>GCS &lt; 15 or other signs of altered mental status (agitated, sleepy, slow to respond, repetitive questions in the ED, other)</t>
+  </si>
+  <si>
+    <t>Not applicable is marked if palpable skull fracture is answered as unclear, no, or missing.</t>
+  </si>
+  <si>
+    <t>Basilar skull fracture: periorbital ecchymosis (raccoon eyes)</t>
+  </si>
+  <si>
+    <t>Basilar skull fracture: retroauricular ecchymosis (battle's sign)</t>
+  </si>
+  <si>
+    <t>Not applicable is marked if other (non-head) substantial injuries is answered as no or missing.</t>
+  </si>
+  <si>
+    <t>This indicates if any head CT was performed regardless of where it was obtained except if the ED head CT was marked as "not interpretable".</t>
+  </si>
+  <si>
+    <t>PatNum</t>
+  </si>
+  <si>
+    <t>Patient Number</t>
+  </si>
+  <si>
+    <t>A randomly generated number that uniquely identifies each patient.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YesNoPV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0   No
+1   Yes
+91 Pre-verbal/Non-verbal</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YesNoLOC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0   No
+1  Yes
+2   Suspected</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YesNo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0   No
+1   Yes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YesNoNA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0   No
+1   Yes
+92 Not applicable</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YesNoUnc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0  No
+1  Yes
+2  Unclear exam</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YesNoClo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0   No/Closed
+1   Yes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>YesNo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+0   No
+1   Yes</t>
+    </r>
+  </si>
+  <si>
+    <t>Not applicable was marked if question of whether patient was given or will patient be given pharmacological sedation for head CT is answered as no, not applicable, or missing.
+More than one reason for pharmacological sedation can be selected for each patient.</t>
+  </si>
+  <si>
+    <t>Finding23</t>
+  </si>
+  <si>
+    <t>Hospitalized for 2 or more nights due to head injury and had TBI on CT</t>
+  </si>
+  <si>
+    <t>Clinically-important TBI was defined as having at least one of the following: (1) neurosurgical procedure performed, (2)  intubated &gt; 24 hours for head trauma,  (3) death due to TBI or in the ED, (4) hospitalized for &gt;= 2 nights due to head injury and having a TBI on CT.</t>
+  </si>
+  <si>
+    <t>The first traumatic head CT of any patient was reviewed in order to determine if there was a TBI on CT.  TBI on CT is defined as any of the traumatic findings (1-23) below, except for skull fracture.  Skull fractures were not regarded as TBIs unless the fracture was depressed by  at least the width of the skull.
+Not applicable is marked if no head CT was performed.</t>
+  </si>
+  <si>
+    <t>As reported by the physician not by the patient/guardian.</t>
+  </si>
+  <si>
+    <t>AMS was defined as a GCS between 3 and 14 or other signs of altered mental status (agitation, repetitive questions, sleepy, slow to respond, or other)</t>
+  </si>
+  <si>
+    <t>Traumatic finding: cerebral contusion</t>
+  </si>
+  <si>
+    <t>Traumatic finding: diastasis of the skull</t>
+  </si>
+  <si>
+    <t>TBI Prediction Rule:</t>
+  </si>
+  <si>
+    <t>TBI Prediction Rule Article Reference:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kuppermann N, Holmes JF, Dayan PS, Hoyle JD, Atabaki SM, Holubkov R, Nadel FM, Monroe D, Stanley RM, Borgialli DA, Badawy MK, Schunk JE, Quayle KS, Mahajan P, Lichenstein R, Lillis KA, Tunik MG, Jacobs ES, Callahan JM, Gorelick MH, Glass TF, Lee LK, Bachman MC, Cooper A, Powell EC, Gerardi MJ, Melville KA, Muizelaar JP, Wisner DH, Zuspan SJ, Dean JM, Wooten-Gorges SL for the Pediatric Emergency Care Applied Research Network (PECARN).  Identifying children at very low risk of clinically-important traumatic brain injuries after blunt head trauma. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lancet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2009:374 1160-70.</t>
+    </r>
+  </si>
+  <si>
+    <t>A prediction rule for identifying children at very low risk of clinically-important TBI was published in Lancet in 2009. The full reference for this publication is provided below. Note that not all variables in the public use dataset were considered for the rule. In addition, the rule is based on the subset of patients who had a total GCS of 14 or 15 and were not missing the primary outcome of clinically-important TBI. The most rigorous attention to data cleaning and verification was given to the subjects and data elements included in the creation of the rule.</t>
+  </si>
+  <si>
+    <t>An attending or fellow physician reviewed all forms.</t>
+  </si>
+  <si>
+    <t>If significant swelling or some other reason limits the physician's ability to assess for a skull fracture "Unclear exam" was marked.
+In the clinical prediction rule, palpable skull fracture and unclear exam were combined.</t>
+  </si>
+  <si>
+    <t>The hospitalization had to be due to the traumatic brain injury and not for social reasons.
+This was defined as a patient having been hospitalized 2 or more nights due to a head injury and also having a TBI on CT.</t>
+  </si>
+  <si>
+    <t>IndAge</t>
+  </si>
+  <si>
+    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: young age</t>
+  </si>
+  <si>
+    <t>Not applicable is marked if a head CT, skull x-ray or head MRI being ordered or obtained is answered as no or missing.
+More than one indication can be selected for each patient.</t>
+  </si>
+  <si>
+    <t>IndAmnesia</t>
+  </si>
+  <si>
+    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: amnesia</t>
+  </si>
+  <si>
+    <t>IndAMS</t>
+  </si>
+  <si>
+    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: decreased mental status</t>
+  </si>
+  <si>
+    <t>IndClinSFx</t>
+  </si>
+  <si>
+    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: clinical evidence of skull fracture</t>
+  </si>
+  <si>
+    <t>IndHA</t>
+  </si>
+  <si>
+    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: headache</t>
+  </si>
+  <si>
+    <t>IndHema</t>
+  </si>
+  <si>
+    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: scalp hematoma</t>
+  </si>
+  <si>
+    <t>IndLOC</t>
+  </si>
+  <si>
+    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: loss of consciousness</t>
+  </si>
+  <si>
+    <t>IndMech</t>
+  </si>
+  <si>
+    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: mechanism</t>
+  </si>
+  <si>
+    <t>IndNeuroD</t>
+  </si>
+  <si>
+    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: neurological deficit (other than mental status)</t>
+  </si>
+  <si>
+    <t>IndRqstMD</t>
+  </si>
+  <si>
+    <t>If a CT is being ordered or obtained  check the most important indications in influencing the decision to obtain a head CT: referring MD request</t>
+  </si>
+  <si>
+    <t>IndRqstParent</t>
+  </si>
+  <si>
+    <t>If a CT is being ordered or obtained  check the most important indications in influencing the decision to obtain a head CT: parental anxiety/request</t>
+  </si>
+  <si>
+    <t>IndRqstTrauma</t>
+  </si>
+  <si>
+    <t>If a CT is being ordered or obtained  check the most important indications in influencing the decision to obtain a head CT: trauma team request</t>
+  </si>
+  <si>
+    <t>IndSeiz</t>
+  </si>
+  <si>
+    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: seizure</t>
+  </si>
+  <si>
+    <t>IndVomit</t>
+  </si>
+  <si>
+    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: vomiting</t>
+  </si>
+  <si>
+    <t>IndXraySFx</t>
+  </si>
+  <si>
+    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: skull fracture on x-ray</t>
+  </si>
+  <si>
+    <t>IndOth</t>
+  </si>
+  <si>
+    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This prospective observational cohort study enrolled children younger than 18 years of age with minor head trauma evaluated in 25 PECARN emergency departments. The goal was to derive and validate two clinical prediction rules to accurately identify children at near-zero risk of clinically important traumatic brain injuries after blunt trauma (one rule for children younger than 2 years, the other for children 2 years and older).  We enrolled subjects presenting within 24 hours of head trauma with Glasgow Coma Scale scores of 14-15. These validated prediction rules identified children at very low risk of clinically important traumatic brain injuries (TBI) for whom CT scans can routinely be obviated. </t>
+  </si>
+  <si>
+    <t>Children presenting within 24 hours of head trauma were included in the public use dataset regardless of GCS score. We excluded children with trivial injury mechanisms defined by ground-level falls or walking or running into stationary objects, and no signs or symptoms of head trauma other than scalp abrasions and lacerations.  Patients were also excluded if they had penetrating trauma, known brain tumors, pre-existing neurological disorders complicating assessment, or neuroimaging at an outside hospital before transfer.  Patients were excluded if they had ventricular shunts or bleeding disorders.</t>
+  </si>
+  <si>
+    <t>Inclusion/Exclusion for Public Use Dataset:</t>
+  </si>
+  <si>
+    <t>Patients were admitted to the hospital at emergency department physician discretion. Records of admitted patients were reviewed by research coordinators and site investigators to assess CT results and presence of ciTBIs. To identify missed traumatic brain injuries, research coordinators
+did standardized telephone surveys of guardians of patients discharged from the emergency department between 7 and 90 days after the emergency department visit. Medical records and imaging results were obtained if a missed traumatic brain injury was suggested at follow-up. If a ciTBI was identified, the patient’s outcome was classified accordingly. If we were unable to contact the patient’s guardian, we reviewed the medical record, emergency department process improvement records, and county morgue records, to ensure that no discharged
+patient was subsequently diagnosed with ciTBI.</t>
+  </si>
+  <si>
+    <t>We defined clinically-important TBI (ciTBI) a priori as death from TBI, neurosurgery, intubation for more than 24 hours for TBI, or hospital admission of two or more nights for theTBI in association with TBI on CT. This outcome was defined to exclude brief intubations for imaging or overnight admission for minor CT findings.  Hospitalizations for social reasons were not included.
+TBI on CT was defined by intracranial hemorrhage or contusion, cerebral edema, traumatic infarction, diffuse axonal injury, shearing injury, sigmoid sinus thrombosis, midline shift of intracranial contents or signs of brain herniation, diastasis of the skull, pneumocephalus, or skull fracture depressed by at least the width of the skull table.</t>
+  </si>
+  <si>
+    <t>Injury Severity based on the injury mechanism classification
+High
+     Motor vehicle collision with patient ejection, 
+      death of another passenger, or rollover
+     Pedestrian or bicyclist without helmet struck
+       by a motorized vehicle
+     Falls of &gt; 5 feet for patients 2 yrs and older
+     Falls of &gt; 3 feet  &lt; 2 yrs
+     Head struck by a high-impact object
+Low
+     Fall from ground level (or fall to ground from
+       standing, walking or running)
+     Walked/ran into stationary object
+Medium
+      Any other mechanism</t>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>back</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>back</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>exclude 3-13
+(only 969)</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Aaron</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>x</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>RES</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>RES</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>RES</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>RES</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAIN RES</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTSed</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTSedAgitate</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTSedAge</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTSedRqst</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>CTSedOth</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>AgeinYears</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>EmplType</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Certification</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -794,1063 +1797,94 @@
 90   Other mechanism
 </t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>InjSev</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1   Low
-2   Moderate
-3   High</t>
-    </r>
-  </si>
-  <si>
-    <t>Severity of injury mechanism</t>
-  </si>
-  <si>
-    <t>Does the parent think the child is acting normally / like themself?</t>
-  </si>
-  <si>
-    <t>Pre-verbal is marked if the patient is too young to speak.  Non-verbal is marked if the patient is intubated or otherwise unable to give an understandable verbal response.  Pre-verbal and non-verbal were determined by the physician.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>LocLen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1   &lt; 5 sec
-2   5 sec - &lt; 1 min
-3   1 -5 min
-4   &gt; 5 min
-92 Not applicable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SeizOcc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1   Immediately on contact
-2   Within 30 minutes of injury
-3   &gt; 30 minutes after injury
-92 Not applicable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>SeizLen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1  &lt; 1 min
-2   1 - &lt; 5 min
-3   5 - 15 min
-4  &gt; 15 min
-92  Not applicable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>HASev</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1   Mild (barely noticeable)
-2   Moderate
-3   Severe (intense)
-92 Not applicable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Start</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1  Before head injury
-2  Within 1 hr of event
-3  1 - 4 hrs after event
-4  &gt; 4 hrs after event
-92  Not applicable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>VomEpi</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1   Once
-2   Twice
-3   &gt; 2 times
-92 Not applicable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Start</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1   Before head injury
-2   Within 1 hr of event
-3  1 - 4 hrs after event
-4   &gt; 4 hrs after event
-92  Not applicable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>VomLast</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1   &lt; 1 hr before ED evaluation
-2   1 -4 hrs before ED evaluation
-3  &gt; 4 hrs before ED evaluation
-92  Not applicable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GCSEye</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1     None
-2     Pain
-3     Verbal
-4    Spontaneous</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GCSVerbal</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1    None
-2    Incomprehensible sounds (moans)
-3    Inappropriate words (cries to pain)
-4    Confused (irritable/cries)
-5    Oriented (coos/babbles)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GCSMotor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1    None
-2    Abnormal extension posturing
-3    Abnormal flexure posturing
-4    Withdraws to pain
-5    Localizes pain (withdraws to touch)
-6    Follow commands (spontaneous
-      movement)</t>
-    </r>
-  </si>
-  <si>
-    <t>Numeric</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>GCSGroup</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1   3 - 13
-2  14 - 15</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>HemLoc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1  Frontal
-2  Occipital
-3  Parietal/Temporal
-92  Not applicable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>HemSz</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1     Small (&lt;1 cm, barely palpable)
-2     Medium (1-3 cm)
-3     Large (&gt;3 cm)
-92   Not applicable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>AgeTwo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1   &lt; 2 years
-2   &gt; = 2 years</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Gender</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1   Male
-2   Female</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Ethn</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1  Hispanic
-2   Non-Hispanic</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Race</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1  White
-2  Black
-3  Asian
-4  American Indian/Alaskan Native
-5  Pacific Islander
-90 Other</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Disp</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1  Home
-2  OR
-3  Admit - general inpatient
-4  Admit short-stay (&lt; 24 hr)/observation unit
-5  ICU
-6  Transferred to another hospital
-7 AMA
-8  Death in ED
-90  Other</t>
-    </r>
-  </si>
-  <si>
-    <t>Duration of loss of consciousness</t>
-  </si>
-  <si>
-    <t>GCS &lt; 15 or other signs of altered mental status (agitated, sleepy, slow to respond, repetitive questions in the ED, other)</t>
-  </si>
-  <si>
-    <t>Not applicable is marked if palpable skull fracture is answered as unclear, no, or missing.</t>
-  </si>
-  <si>
-    <t>Basilar skull fracture: periorbital ecchymosis (raccoon eyes)</t>
-  </si>
-  <si>
-    <t>Basilar skull fracture: retroauricular ecchymosis (battle's sign)</t>
-  </si>
-  <si>
-    <t>Not applicable is marked if other (non-head) substantial injuries is answered as no or missing.</t>
-  </si>
-  <si>
-    <t>This indicates if any head CT was performed regardless of where it was obtained except if the ED head CT was marked as "not interpretable".</t>
-  </si>
-  <si>
-    <t>PatNum</t>
-  </si>
-  <si>
-    <t>Patient Number</t>
-  </si>
-  <si>
-    <t>A randomly generated number that uniquely identifies each patient.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>YesNoPV</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0   No
-1   Yes
-91 Pre-verbal/Non-verbal</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>YesNoLOC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0   No
-1  Yes
-2   Suspected</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>YesNo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0   No
-1   Yes</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>YesNoNA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0   No
-1   Yes
-92 Not applicable</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>YesNoUnc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0  No
-1  Yes
-2  Unclear exam</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>YesNoClo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0   No/Closed
-1   Yes</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>YesNo</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0   No
-1   Yes</t>
-    </r>
-  </si>
-  <si>
-    <t>Not applicable was marked if question of whether patient was given or will patient be given pharmacological sedation for head CT is answered as no, not applicable, or missing.
-More than one reason for pharmacological sedation can be selected for each patient.</t>
-  </si>
-  <si>
-    <t>Finding23</t>
-  </si>
-  <si>
-    <t>Hospitalized for 2 or more nights due to head injury and had TBI on CT</t>
-  </si>
-  <si>
-    <t>Clinically-important TBI was defined as having at least one of the following: (1) neurosurgical procedure performed, (2)  intubated &gt; 24 hours for head trauma,  (3) death due to TBI or in the ED, (4) hospitalized for &gt;= 2 nights due to head injury and having a TBI on CT.</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>High_impact_InjSev</t>
-  </si>
-  <si>
-    <t>The first traumatic head CT of any patient was reviewed in order to determine if there was a TBI on CT.  TBI on CT is defined as any of the traumatic findings (1-23) below, except for skull fracture.  Skull fractures were not regarded as TBIs unless the fracture was depressed by  at least the width of the skull.
-Not applicable is marked if no head CT was performed.</t>
-  </si>
-  <si>
-    <t>As reported by the physician not by the patient/guardian.</t>
-  </si>
-  <si>
-    <t>AMS was defined as a GCS between 3 and 14 or other signs of altered mental status (agitation, repetitive questions, sleepy, slow to respond, or other)</t>
-  </si>
-  <si>
-    <t>Traumatic finding: cerebral contusion</t>
-  </si>
-  <si>
-    <t>Traumatic finding: diastasis of the skull</t>
-  </si>
-  <si>
-    <t>TBI Prediction Rule:</t>
-  </si>
-  <si>
-    <t>TBI Prediction Rule Article Reference:</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Kuppermann N, Holmes JF, Dayan PS, Hoyle JD, Atabaki SM, Holubkov R, Nadel FM, Monroe D, Stanley RM, Borgialli DA, Badawy MK, Schunk JE, Quayle KS, Mahajan P, Lichenstein R, Lillis KA, Tunik MG, Jacobs ES, Callahan JM, Gorelick MH, Glass TF, Lee LK, Bachman MC, Cooper A, Powell EC, Gerardi MJ, Melville KA, Muizelaar JP, Wisner DH, Zuspan SJ, Dean JM, Wooten-Gorges SL for the Pediatric Emergency Care Applied Research Network (PECARN).  Identifying children at very low risk of clinically-important traumatic brain injuries after blunt head trauma. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lancet</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 2009:374 1160-70.</t>
-    </r>
-  </si>
-  <si>
-    <t>A prediction rule for identifying children at very low risk of clinically-important TBI was published in Lancet in 2009. The full reference for this publication is provided below. Note that not all variables in the public use dataset were considered for the rule. In addition, the rule is based on the subset of patients who had a total GCS of 14 or 15 and were not missing the primary outcome of clinically-important TBI. The most rigorous attention to data cleaning and verification was given to the subjects and data elements included in the creation of the rule.</t>
-  </si>
-  <si>
-    <t>An attending or fellow physician reviewed all forms.</t>
-  </si>
-  <si>
-    <t>If significant swelling or some other reason limits the physician's ability to assess for a skull fracture "Unclear exam" was marked.
-In the clinical prediction rule, palpable skull fracture and unclear exam were combined.</t>
-  </si>
-  <si>
-    <t>The hospitalization had to be due to the traumatic brain injury and not for social reasons.
-This was defined as a patient having been hospitalized 2 or more nights due to a head injury and also having a TBI on CT.</t>
-  </si>
-  <si>
-    <t>IndAge</t>
-  </si>
-  <si>
-    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: young age</t>
-  </si>
-  <si>
-    <t>Not applicable is marked if a head CT, skull x-ray or head MRI being ordered or obtained is answered as no or missing.
-More than one indication can be selected for each patient.</t>
-  </si>
-  <si>
-    <t>IndAmnesia</t>
-  </si>
-  <si>
-    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: amnesia</t>
-  </si>
-  <si>
-    <t>IndAMS</t>
-  </si>
-  <si>
-    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: decreased mental status</t>
-  </si>
-  <si>
-    <t>IndClinSFx</t>
-  </si>
-  <si>
-    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: clinical evidence of skull fracture</t>
-  </si>
-  <si>
-    <t>IndHA</t>
-  </si>
-  <si>
-    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: headache</t>
-  </si>
-  <si>
-    <t>IndHema</t>
-  </si>
-  <si>
-    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: scalp hematoma</t>
-  </si>
-  <si>
-    <t>IndLOC</t>
-  </si>
-  <si>
-    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: loss of consciousness</t>
-  </si>
-  <si>
-    <t>IndMech</t>
-  </si>
-  <si>
-    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: mechanism</t>
-  </si>
-  <si>
-    <t>IndNeuroD</t>
-  </si>
-  <si>
-    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: neurological deficit (other than mental status)</t>
-  </si>
-  <si>
-    <t>IndRqstMD</t>
-  </si>
-  <si>
-    <t>If a CT is being ordered or obtained  check the most important indications in influencing the decision to obtain a head CT: referring MD request</t>
-  </si>
-  <si>
-    <t>IndRqstParent</t>
-  </si>
-  <si>
-    <t>If a CT is being ordered or obtained  check the most important indications in influencing the decision to obtain a head CT: parental anxiety/request</t>
-  </si>
-  <si>
-    <t>IndRqstTrauma</t>
-  </si>
-  <si>
-    <t>If a CT is being ordered or obtained  check the most important indications in influencing the decision to obtain a head CT: trauma team request</t>
-  </si>
-  <si>
-    <t>IndSeiz</t>
-  </si>
-  <si>
-    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: seizure</t>
-  </si>
-  <si>
-    <t>IndVomit</t>
-  </si>
-  <si>
-    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: vomiting</t>
-  </si>
-  <si>
-    <t>IndXraySFx</t>
-  </si>
-  <si>
-    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: skull fracture on x-ray</t>
-  </si>
-  <si>
-    <t>IndOth</t>
-  </si>
-  <si>
-    <t>If a CT is being ordered or obtained check the most important indications in influencing the decision to obtain a head CT: other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This prospective observational cohort study enrolled children younger than 18 years of age with minor head trauma evaluated in 25 PECARN emergency departments. The goal was to derive and validate two clinical prediction rules to accurately identify children at near-zero risk of clinically important traumatic brain injuries after blunt trauma (one rule for children younger than 2 years, the other for children 2 years and older).  We enrolled subjects presenting within 24 hours of head trauma with Glasgow Coma Scale scores of 14-15. These validated prediction rules identified children at very low risk of clinically important traumatic brain injuries (TBI) for whom CT scans can routinely be obviated. </t>
-  </si>
-  <si>
-    <t>Children presenting within 24 hours of head trauma were included in the public use dataset regardless of GCS score. We excluded children with trivial injury mechanisms defined by ground-level falls or walking or running into stationary objects, and no signs or symptoms of head trauma other than scalp abrasions and lacerations.  Patients were also excluded if they had penetrating trauma, known brain tumors, pre-existing neurological disorders complicating assessment, or neuroimaging at an outside hospital before transfer.  Patients were excluded if they had ventricular shunts or bleeding disorders.</t>
-  </si>
-  <si>
-    <t>Inclusion/Exclusion for Public Use Dataset:</t>
-  </si>
-  <si>
-    <t>Patients were admitted to the hospital at emergency department physician discretion. Records of admitted patients were reviewed by research coordinators and site investigators to assess CT results and presence of ciTBIs. To identify missed traumatic brain injuries, research coordinators
-did standardized telephone surveys of guardians of patients discharged from the emergency department between 7 and 90 days after the emergency department visit. Medical records and imaging results were obtained if a missed traumatic brain injury was suggested at follow-up. If a ciTBI was identified, the patient’s outcome was classified accordingly. If we were unable to contact the patient’s guardian, we reviewed the medical record, emergency department process improvement records, and county morgue records, to ensure that no discharged
-patient was subsequently diagnosed with ciTBI.</t>
-  </si>
-  <si>
-    <t>We defined clinically-important TBI (ciTBI) a priori as death from TBI, neurosurgery, intubation for more than 24 hours for TBI, or hospital admission of two or more nights for theTBI in association with TBI on CT. This outcome was defined to exclude brief intubations for imaging or overnight admission for minor CT findings.  Hospitalizations for social reasons were not included.
-TBI on CT was defined by intracranial hemorrhage or contusion, cerebral edema, traumatic infarction, diffuse axonal injury, shearing injury, sigmoid sinus thrombosis, midline shift of intracranial contents or signs of brain herniation, diastasis of the skull, pneumocephalus, or skull fracture depressed by at least the width of the skull table.</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Amnesia_verb</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOCSeparate</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clinical suspicion for alcohol or drug intoxication (not by laboratory testing)?</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Drugs</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>HAStart</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>HASeverity</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>VomitLast</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seiz</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>HemaSize</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeuroD</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>VomitStart</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>VomitNbr</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>HemaLoc</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>SeizLen</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>SeizOccur</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gender</t>
+    <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
     <t>InjuryMech</t>
-  </si>
-  <si>
-    <t>Injury Severity based on the injury mechanism classification
-High
-     Motor vehicle collision with patient ejection, 
-      death of another passenger, or rollover
-     Pedestrian or bicyclist without helmet struck
-       by a motorized vehicle
-     Falls of &gt; 5 feet for patients 2 yrs and older
-     Falls of &gt; 3 feet  &lt; 2 yrs
-     Head struck by a high-impact object
-Low
-     Fall from ground level (or fall to ground from
-       standing, walking or running)
-     Walked/ran into stationary object
-Medium
-      Any other mechanism</t>
-  </si>
-  <si>
-    <t>x</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>x</t>
+    <t>ActNorm</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>back</t>
+    <t>SFxPalp</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>back</t>
+    <t>FontBulg</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
   <si>
-    <t>exclude 3-13
-(only 969)</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Aaron</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>x</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>RES</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>RES</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>RES</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>RES</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>MAIN RES</t>
+    <t>AgeTwoPlus</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -2126,6 +2160,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2158,9 +2195,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2468,8 +2502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2482,82 +2516,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="44"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="45"/>
     </row>
     <row r="2" spans="1:5" ht="81" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="37" t="s">
-        <v>318</v>
-      </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
+        <v>131</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>289</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
     </row>
     <row r="3" spans="1:5" ht="77.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>319</v>
-      </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
+        <v>291</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>290</v>
+      </c>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
     </row>
     <row r="4" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>160</v>
-      </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
+        <v>132</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
     </row>
     <row r="5" spans="1:5" ht="111" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" s="45" t="s">
-        <v>322</v>
-      </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="47"/>
+        <v>135</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>293</v>
+      </c>
+      <c r="C5" s="47"/>
+      <c r="D5" s="48"/>
     </row>
     <row r="6" spans="1:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>321</v>
-      </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
+        <v>134</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>292</v>
+      </c>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
     </row>
     <row r="7" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>281</v>
-      </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
+        <v>249</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>252</v>
+      </c>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
     </row>
     <row r="8" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>280</v>
-      </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="40"/>
+        <v>250</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>251</v>
+      </c>
+      <c r="C8" s="40"/>
+      <c r="D8" s="41"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="29"/>
@@ -2579,1888 +2613,1888 @@
         <v>2</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>222</v>
+        <v>195</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="33" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>258</v>
+        <v>230</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="99" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>3</v>
+        <v>320</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>223</v>
+        <v>196</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>282</v>
+        <v>253</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="99" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>4</v>
+        <v>321</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>225</v>
+        <v>198</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>224</v>
+        <v>197</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="1" t="s">
-        <v>326</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="346.5" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>323</v>
+        <v>340</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>226</v>
+        <v>322</v>
       </c>
       <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:5" ht="264" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>272</v>
+        <v>323</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>228</v>
+        <v>200</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>227</v>
+        <v>199</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>324</v>
+        <v>294</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="10" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>6</v>
+        <v>324</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>7</v>
+        <v>325</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>180</v>
+        <v>153</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:5" ht="99" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>231</v>
+        <v>203</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>9</v>
+        <v>331</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>219</v>
+        <v>192</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>10</v>
+        <v>338</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>232</v>
+        <v>204</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="99" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
-        <v>12</v>
+        <v>337</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>14</v>
+        <v>341</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>181</v>
+        <v>154</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>16</v>
+        <v>329</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>234</v>
+        <v>206</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="99" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>17</v>
+        <v>328</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>235</v>
+        <v>207</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>19</v>
+        <v>335</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>125</v>
+        <v>99</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>236</v>
+        <v>208</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>171</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="99" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>20</v>
+        <v>334</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>237</v>
+        <v>209</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>171</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>21</v>
+        <v>330</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>171</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D32" s="7"/>
     </row>
     <row r="33" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D33" s="7"/>
     </row>
     <row r="34" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D34" s="7"/>
     </row>
     <row r="35" spans="1:6" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>218</v>
+        <v>191</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="1" t="s">
-        <v>327</v>
+        <v>297</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>217</v>
+        <v>190</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="1" t="s">
-        <v>328</v>
+        <v>298</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="132" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>216</v>
+        <v>189</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="1" t="s">
-        <v>327</v>
+        <v>297</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="D38" s="21"/>
     </row>
     <row r="39" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="D39" s="7"/>
-      <c r="E39" s="48" t="s">
-        <v>329</v>
+      <c r="E39" s="37" t="s">
+        <v>299</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>330</v>
+        <v>300</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>252</v>
+        <v>224</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>275</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="66" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="66" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="10" customFormat="1" ht="66" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="99" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
-        <v>39</v>
+        <v>342</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>283</v>
+        <v>254</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="66" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>253</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>42</v>
+        <v>343</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>266</v>
+        <v>238</v>
       </c>
       <c r="D48" s="7"/>
     </row>
     <row r="49" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>172</v>
+        <v>145</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D49" s="7"/>
     </row>
     <row r="50" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>254</v>
+        <v>226</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>255</v>
+        <v>227</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
-        <v>51</v>
+        <v>336</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
-        <v>53</v>
+        <v>332</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D58" s="7"/>
     </row>
     <row r="59" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
-        <v>62</v>
+        <v>333</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D65" s="7"/>
     </row>
     <row r="66" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>145</v>
+        <v>119</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>146</v>
+        <v>120</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D69" s="7" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D71" s="7"/>
     </row>
     <row r="72" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D75" s="7" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A76" s="12" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D76" s="7" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A77" s="12" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A78" s="12" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
-        <v>77</v>
+        <v>327</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>156</v>
+        <v>326</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D79" s="7"/>
     </row>
     <row r="80" spans="1:5" ht="132" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A81" s="34" t="s">
-        <v>285</v>
+        <v>256</v>
       </c>
       <c r="B81" s="36" t="s">
-        <v>286</v>
+        <v>257</v>
       </c>
       <c r="C81" s="34" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D81" s="35" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="E81" s="33" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="82" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A82" s="34" t="s">
-        <v>288</v>
+        <v>259</v>
       </c>
       <c r="B82" s="36" t="s">
-        <v>289</v>
+        <v>260</v>
       </c>
       <c r="C82" s="34" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D82" s="35" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="E82" s="33" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="83" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A83" s="34" t="s">
-        <v>290</v>
+        <v>261</v>
       </c>
       <c r="B83" s="36" t="s">
-        <v>291</v>
+        <v>262</v>
       </c>
       <c r="C83" s="34" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D83" s="35" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="E83" s="33" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="84" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A84" s="34" t="s">
-        <v>292</v>
+        <v>263</v>
       </c>
       <c r="B84" s="36" t="s">
-        <v>293</v>
+        <v>264</v>
       </c>
       <c r="C84" s="34" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D84" s="35" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="E84" s="33" t="s">
-        <v>331</v>
+        <v>301</v>
       </c>
     </row>
     <row r="85" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A85" s="34" t="s">
-        <v>294</v>
+        <v>265</v>
       </c>
       <c r="B85" s="36" t="s">
+        <v>266</v>
+      </c>
+      <c r="C85" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="D85" s="35" t="s">
+        <v>258</v>
+      </c>
+      <c r="E85" s="33" t="s">
         <v>295</v>
-      </c>
-      <c r="C85" s="34" t="s">
-        <v>264</v>
-      </c>
-      <c r="D85" s="35" t="s">
-        <v>287</v>
-      </c>
-      <c r="E85" s="33" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="86" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A86" s="34" t="s">
-        <v>296</v>
+        <v>267</v>
       </c>
       <c r="B86" s="36" t="s">
-        <v>297</v>
+        <v>268</v>
       </c>
       <c r="C86" s="34" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D86" s="35" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="E86" s="33" t="s">
-        <v>332</v>
+        <v>302</v>
       </c>
     </row>
     <row r="87" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A87" s="34" t="s">
-        <v>298</v>
+        <v>269</v>
       </c>
       <c r="B87" s="36" t="s">
-        <v>299</v>
+        <v>270</v>
       </c>
       <c r="C87" s="34" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D87" s="35" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="E87" s="33" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="88" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A88" s="34" t="s">
-        <v>300</v>
+        <v>271</v>
       </c>
       <c r="B88" s="36" t="s">
-        <v>301</v>
+        <v>272</v>
       </c>
       <c r="C88" s="34" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D88" s="35" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="E88" s="33" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="89" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A89" s="34" t="s">
-        <v>302</v>
+        <v>273</v>
       </c>
       <c r="B89" s="36" t="s">
-        <v>303</v>
+        <v>274</v>
       </c>
       <c r="C89" s="34" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D89" s="35" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="E89" s="33" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="90" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A90" s="34" t="s">
-        <v>304</v>
+        <v>275</v>
       </c>
       <c r="B90" s="36" t="s">
-        <v>305</v>
+        <v>276</v>
       </c>
       <c r="C90" s="34" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D90" s="35" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="E90" s="33" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="91" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A91" s="34" t="s">
-        <v>306</v>
+        <v>277</v>
       </c>
       <c r="B91" s="36" t="s">
-        <v>307</v>
+        <v>278</v>
       </c>
       <c r="C91" s="34" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D91" s="35" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="E91" s="33" t="s">
-        <v>333</v>
+        <v>303</v>
       </c>
     </row>
     <row r="92" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A92" s="34" t="s">
-        <v>308</v>
+        <v>279</v>
       </c>
       <c r="B92" s="36" t="s">
-        <v>309</v>
+        <v>280</v>
       </c>
       <c r="C92" s="34" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D92" s="35" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="E92" s="33" t="s">
-        <v>333</v>
+        <v>303</v>
       </c>
     </row>
     <row r="93" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A93" s="34" t="s">
-        <v>310</v>
+        <v>281</v>
       </c>
       <c r="B93" s="36" t="s">
-        <v>311</v>
+        <v>282</v>
       </c>
       <c r="C93" s="34" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D93" s="35" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="E93" s="33" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="94" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A94" s="34" t="s">
-        <v>312</v>
+        <v>283</v>
       </c>
       <c r="B94" s="36" t="s">
-        <v>313</v>
+        <v>284</v>
       </c>
       <c r="C94" s="34" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D94" s="35" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="E94" s="33" t="s">
-        <v>334</v>
+        <v>304</v>
       </c>
     </row>
     <row r="95" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A95" s="34" t="s">
-        <v>314</v>
+        <v>285</v>
       </c>
       <c r="B95" s="36" t="s">
-        <v>315</v>
+        <v>286</v>
       </c>
       <c r="C95" s="34" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D95" s="35" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="E95" s="33" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="96" spans="1:5" s="33" customFormat="1" ht="99" x14ac:dyDescent="0.3">
       <c r="A96" s="34" t="s">
-        <v>316</v>
+        <v>287</v>
       </c>
       <c r="B96" s="36" t="s">
-        <v>317</v>
+        <v>288</v>
       </c>
       <c r="C96" s="34" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D96" s="35" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
       <c r="E96" s="33" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
-        <v>79</v>
+        <v>314</v>
       </c>
       <c r="B97" s="32" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="C97" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>335</v>
+        <v>305</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
-        <v>80</v>
+        <v>315</v>
       </c>
       <c r="B98" s="32" t="s">
-        <v>215</v>
+        <v>188</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
-        <v>81</v>
+        <v>316</v>
       </c>
       <c r="B99" s="32" t="s">
-        <v>213</v>
+        <v>186</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
-        <v>82</v>
+        <v>317</v>
       </c>
       <c r="B100" s="32" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
-        <v>83</v>
+        <v>318</v>
       </c>
       <c r="B101" s="32" t="s">
-        <v>214</v>
+        <v>187</v>
       </c>
       <c r="C101" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>268</v>
+        <v>240</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>336</v>
+        <v>306</v>
       </c>
     </row>
     <row r="102" spans="1:5" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A102" s="6" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="B102" s="32" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="D102" s="7" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
     </row>
     <row r="103" spans="1:5" s="10" customFormat="1" ht="33" x14ac:dyDescent="0.3">
       <c r="A103" s="6" t="s">
-        <v>86</v>
+        <v>319</v>
       </c>
       <c r="B103" s="32" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="D103" s="7" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
     </row>
     <row r="104" spans="1:5" s="10" customFormat="1" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A104" s="6" t="s">
-        <v>87</v>
+        <v>344</v>
       </c>
       <c r="B104" s="32" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="D104" s="7" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A105" s="6" t="s">
-        <v>89</v>
+        <v>339</v>
       </c>
       <c r="B105" s="32" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="D105" s="7"/>
     </row>
     <row r="106" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A106" s="6" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="B106" s="32" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
       <c r="D106" s="7" t="s">
-        <v>274</v>
+        <v>245</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>337</v>
+        <v>307</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A107" s="6" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="B107" s="32" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>249</v>
+        <v>221</v>
       </c>
       <c r="D107" s="7" t="s">
-        <v>274</v>
+        <v>245</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>338</v>
+        <v>308</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A108" s="6" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="B108" s="32" t="s">
-        <v>189</v>
+        <v>162</v>
       </c>
       <c r="C108" s="9" t="s">
-        <v>267</v>
+        <v>239</v>
       </c>
       <c r="D108" s="7"/>
       <c r="E108" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A109" s="6" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="B109" s="32" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>250</v>
+        <v>222</v>
       </c>
       <c r="D109" s="15"/>
       <c r="E109" s="1" t="s">
-        <v>332</v>
+        <v>302</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A110" s="6" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="B110" s="32" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="C110" s="9" t="s">
-        <v>267</v>
+        <v>239</v>
       </c>
       <c r="D110" s="7" t="s">
-        <v>257</v>
+        <v>229</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A111" s="6" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="B111" s="32" t="s">
-        <v>191</v>
+        <v>164</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D111" s="7" t="s">
-        <v>192</v>
+        <v>165</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>337</v>
+        <v>307</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="132" x14ac:dyDescent="0.3">
       <c r="A112" s="6" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="B112" s="32" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D112" s="7" t="s">
-        <v>273</v>
+        <v>244</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>209</v>
+        <v>182</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D113" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A114" s="6" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>276</v>
+        <v>247</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D114" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>332</v>
+        <v>302</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A115" s="6" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D115" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>338</v>
+        <v>308</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A116" s="6" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D116" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A117" s="6" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>277</v>
+        <v>248</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D117" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A118" s="6" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D118" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A119" s="6" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>205</v>
+        <v>178</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D119" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A120" s="6" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D120" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>334</v>
+        <v>304</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A121" s="6" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D121" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>334</v>
+        <v>304</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A122" s="6" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>202</v>
+        <v>175</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D122" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>334</v>
+        <v>304</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A123" s="6" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>201</v>
+        <v>174</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D123" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
-        <v>110</v>
+        <v>84</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>200</v>
+        <v>173</v>
       </c>
       <c r="C124" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D124" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>338</v>
+        <v>308</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>199</v>
+        <v>172</v>
       </c>
       <c r="C125" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D125" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>337</v>
+        <v>307</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A126" s="6" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="C126" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D126" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>336</v>
+        <v>306</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
-        <v>212</v>
+        <v>185</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="C127" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D127" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>336</v>
+        <v>306</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A128" s="6" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D128" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A129" s="6" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="C129" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D129" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>337</v>
+        <v>307</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="66" x14ac:dyDescent="0.3">
       <c r="A130" s="6" t="s">
-        <v>269</v>
+        <v>241</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>194</v>
+        <v>167</v>
       </c>
       <c r="C130" s="6" t="s">
-        <v>264</v>
+        <v>236</v>
       </c>
       <c r="D130" s="16" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D131" s="7"/>
       <c r="E131" s="1" t="s">
-        <v>339</v>
+        <v>309</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
-        <v>117</v>
+        <v>91</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>210</v>
+        <v>183</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D132" s="7"/>
       <c r="E132" s="1" t="s">
-        <v>325</v>
+        <v>295</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="99" x14ac:dyDescent="0.3">
       <c r="A133" s="6" t="s">
-        <v>118</v>
+        <v>92</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>270</v>
+        <v>242</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D133" s="7" t="s">
-        <v>284</v>
+        <v>255</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>341</v>
+        <v>311</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A134" s="6" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>211</v>
+        <v>184</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D134" s="7"/>
       <c r="E134" s="1" t="s">
-        <v>340</v>
+        <v>310</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A135" s="6" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D135" s="7"/>
       <c r="E135" s="1" t="s">
-        <v>342</v>
+        <v>312</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="99" x14ac:dyDescent="0.3">
       <c r="A136" s="6" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>263</v>
+        <v>235</v>
       </c>
       <c r="D136" s="7" t="s">
-        <v>271</v>
+        <v>243</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>343</v>
+        <v>313</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>